<commit_message>
new studies and robustness cycles analysis
</commit_message>
<xml_diff>
--- a/results/pseudomonas_putida/Carbon_Study/pseudomonas_carbon_source_functional_composition.xlsx
+++ b/results/pseudomonas_putida/Carbon_Study/pseudomonas_carbon_source_functional_composition.xlsx
@@ -7,14 +7,14 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_cit_e-7.44-iModulon" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_cit_e-7.44-Subsystem" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_fer_e-2.91-iModulon" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_fer_e-2.91-Subsystem" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_glc_e-7.44-iModulon" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_glc_e-7.44-Subsystem" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_ser__L_e-14.88-iModulon" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_ser__L_e-14.88-Subsystem" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_cit_e7.44-iModulon" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_cit_e7.44-Subsystem" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_fer_e2.91-iModulon" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_fer_e2.91-Subsystem" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_glc_e7.44-iModulon" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_glc_e7.44-Subsystem" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_ser__L_e14.88-iModulon" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="m9-EX_ser__L_e14.88-Subsystem" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>